<commit_message>
updated with summer salary
</commit_message>
<xml_diff>
--- a/Budget/BudgetOverview.xlsx
+++ b/Budget/BudgetOverview.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Budget</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Internship costs</t>
+  </si>
+  <si>
+    <t>Summer salary</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="31" x14ac:dyDescent="0.35"/>
@@ -433,7 +436,7 @@
       </c>
       <c r="E4" s="1" t="str">
         <f>CONCATENATE("Total: $", SUM(E5:E75))</f>
-        <v>Total: $2345000</v>
+        <v>Total: $1451665</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -444,7 +447,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -462,8 +465,7 @@
         <v>30000</v>
       </c>
       <c r="C6" s="1">
-        <f>C5</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1">
         <f>D5</f>
@@ -471,7 +473,7 @@
       </c>
       <c r="E6" s="2">
         <f>B6*C6*D6</f>
-        <v>1800000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -482,14 +484,15 @@
         <v>2000</v>
       </c>
       <c r="C7" s="1">
-        <v>30</v>
+        <f>C6</f>
+        <v>15</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
       <c r="E7" s="2">
         <f>B7*C7*D7</f>
-        <v>120000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -509,14 +512,14 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="2">
         <f>B9*D9</f>
-        <v>125000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -527,7 +530,8 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>30</v>
+        <f>C7</f>
+        <v>15</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -538,7 +542,20 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <f>ROUND(75000/9,0)</f>
+        <v>8333</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <f>B11*D11</f>
+        <v>41665</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E12" s="2"/>

</xml_diff>